<commit_message>
Deploying to gh-pages from @ WWF-Sweden/ITR-tool@8084c4d53afa8b854e87237df10cbcf42600cad6 🚀
</commit_message>
<xml_diff>
--- a/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
+++ b/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mountainrambler\SBTi\SBTi-finance-tool\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daanm\Documents\temp\SBTi\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3473014C-3352-4A89-AE1D-59AB3636BE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="11_BCCFA2BD0AFE4771E24C6D0DBC87A6ED4B30D22F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{35A3BBCA-F2EF-46A8-B156-4D9ACA454480}"/>
   <bookViews>
-    <workbookView xWindow="32025" yWindow="3225" windowWidth="38700" windowHeight="15285" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
     <sheet name="target_data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>company_name</t>
   </si>
@@ -199,25 +199,13 @@
   </si>
   <si>
     <t>Steel</t>
-  </si>
-  <si>
-    <t>target_ids</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,9 +300,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:Q120" totalsRowShown="0">
-  <autoFilter ref="A1:Q120" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:P120" totalsRowShown="0">
+  <autoFilter ref="A1:P120" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="target_type"/>
@@ -331,7 +319,6 @@
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="base_year_ghg_s2"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="base_year_ghg_s3"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="achieved_reduction"/>
-    <tableColumn id="17" xr3:uid="{5F0CB71F-8752-4977-A490-27DCA30723FC}" name="target_ids"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -606,20 +593,20 @@
       <selection activeCell="K2" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="21.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -725,7 +712,7 @@
         <v>990719858</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -791,25 +778,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="4" width="21.109375" customWidth="1"/>
-    <col min="6" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="4" width="21.140625" customWidth="1"/>
+    <col min="6" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="15" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -858,11 +845,8 @@
       <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -902,11 +886,8 @@
       <c r="P2">
         <v>0</v>
       </c>
-      <c r="Q2" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -949,11 +930,9 @@
       <c r="P3">
         <v>0.1</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -998,9 +977,6 @@
       </c>
       <c r="P4">
         <v>0.1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1013,21 +989,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100DEE3DD05F1781645A88261586288E143" ma:contentTypeVersion="8" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="10141bd3b7df6929ac2aab0d38ace983">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84fd47fe-9509-4b60-beed-e31c94bc7d6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="679635ba64e6b0b974d32fba01d99d42" ns2:_="">
     <xsd:import namespace="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
@@ -1199,37 +1160,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}"/>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ WWF-Sweden/ITR-tool@1032016604f2985c92123a5958e260b9ef1bc956 🚀
</commit_message>
<xml_diff>
--- a/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
+++ b/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daanm\Documents\temp\SBTi\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mountainrambler\ITR\ITR-tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_BCCFA2BD0AFE4771E24C6D0DBC87A6ED4B30D22F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{35A3BBCA-F2EF-46A8-B156-4D9ACA454480}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE29F8-0C6F-4264-AD05-34045B75FE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46485" yWindow="3765" windowWidth="32310" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
     <sheet name="target_data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>company_name</t>
   </si>
@@ -66,9 +66,6 @@
     <t>sector</t>
   </si>
   <si>
-    <t>ghg_s1s2</t>
-  </si>
-  <si>
     <t>ghg_s3</t>
   </si>
   <si>
@@ -199,13 +196,43 @@
   </si>
   <si>
     <t>Steel</t>
+  </si>
+  <si>
+    <t>statement_date</t>
+  </si>
+  <si>
+    <t>target_ids</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>ghg_s1</t>
+  </si>
+  <si>
+    <t>ghg_s2</t>
+  </si>
+  <si>
+    <t>s3_category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +244,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -242,9 +275,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -274,9 +308,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q51" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:Q51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R51" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:R51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="isic"/>
@@ -287,7 +321,8 @@
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="industry_level_3"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="industry_level_4"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="sector"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ghg_s1s2"/>
+    <tableColumn id="14" xr3:uid="{4E3A16A5-1D49-4E34-85C1-76B963C0C39B}" name="ghg_s1"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ghg_s2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ghg_s3"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="company_revenue"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="company_market_cap"/>
@@ -300,14 +335,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:P120" totalsRowShown="0">
-  <autoFilter ref="A1:P120" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:S121" totalsRowShown="0">
+  <autoFilter ref="A1:S121" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="target_type"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="intensity_metric"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="scope"/>
+    <tableColumn id="19" xr3:uid="{9248934B-75D3-4E38-B527-74646CCCA9CA}" name="s3_category"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="coverage_s1"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="coverage_s2"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="coverage_s3"/>
@@ -315,10 +351,12 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="base_year"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="end_year"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="start_year"/>
+    <tableColumn id="17" xr3:uid="{402ACC87-EC14-4797-B51B-7DC99260B94B}" name="statement_date"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="base_year_ghg_s1"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="base_year_ghg_s2"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="base_year_ghg_s3"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="achieved_reduction"/>
+    <tableColumn id="18" xr3:uid="{9D6E6BD8-AF52-471F-81F4-E934F549E268}" name="target_ids"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -587,26 +625,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="21.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="21.5546875" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -638,130 +676,139 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
-        <v>17</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2">
+        <v>228332160</v>
+      </c>
+      <c r="L2">
+        <v>188332160</v>
+      </c>
+      <c r="M2">
+        <v>61888133</v>
+      </c>
+      <c r="N2">
+        <v>7370536918</v>
+      </c>
+      <c r="O2">
+        <v>7318942238</v>
+      </c>
+      <c r="P2">
+        <v>24392175674</v>
+      </c>
+      <c r="Q2">
+        <v>21337139</v>
+      </c>
+      <c r="R2">
+        <v>990719858</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>25</v>
-      </c>
-      <c r="K2">
-        <v>458332160</v>
-      </c>
-      <c r="L2">
-        <v>61888133</v>
-      </c>
-      <c r="M2">
-        <v>7370536918</v>
-      </c>
-      <c r="N2">
-        <v>7318942238</v>
-      </c>
-      <c r="O2">
-        <v>24392175674</v>
-      </c>
-      <c r="P2">
-        <v>21337139</v>
-      </c>
-      <c r="Q2">
-        <v>990719858</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>26</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>33</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
       </c>
       <c r="K3">
         <v>13266889.880000001</v>
       </c>
       <c r="L3">
+        <v>3266889</v>
+      </c>
+      <c r="M3">
         <v>18413448.829999998</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>2795781568</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>3615211346</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>3620291185</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>43581896.049999997</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>463981837.19999999</v>
       </c>
     </row>
@@ -776,27 +823,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="4" width="21.140625" customWidth="1"/>
-    <col min="6" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="4" width="21.109375" customWidth="1"/>
+    <col min="7" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="13" max="14" width="21" customWidth="1"/>
+    <col min="15" max="17" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -804,182 +851,259 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
         <v>44</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>45</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
-        <v>48</v>
+      <c r="S1" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <v>0.95</v>
       </c>
       <c r="G2">
         <v>0.95</v>
       </c>
-      <c r="I2">
+      <c r="H2">
+        <v>0.95</v>
+      </c>
+      <c r="J2">
         <v>0.35</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2020</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>2035</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>2020</v>
       </c>
-      <c r="M2">
+      <c r="N2">
+        <v>2024</v>
+      </c>
+      <c r="O2">
         <v>458332160</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>61888133</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>0</v>
       </c>
+      <c r="S2" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.7</v>
+      </c>
+      <c r="J3">
+        <v>0.25</v>
+      </c>
+      <c r="K3">
+        <v>2019</v>
+      </c>
+      <c r="L3">
+        <v>2030</v>
+      </c>
+      <c r="M3">
+        <v>2019</v>
+      </c>
+      <c r="N3" s="2">
+        <v>45200</v>
+      </c>
+      <c r="O3">
+        <v>6128444</v>
+      </c>
+      <c r="P3">
+        <v>6128444</v>
+      </c>
+      <c r="Q3">
+        <v>16913448.829999998</v>
+      </c>
+      <c r="R3">
+        <v>0.1</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4">
+        <v>0.85</v>
+      </c>
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+      <c r="K4">
+        <v>2019</v>
+      </c>
+      <c r="L4">
+        <v>2030</v>
+      </c>
+      <c r="M4">
+        <v>2019</v>
+      </c>
+      <c r="N4">
+        <v>2024</v>
+      </c>
+      <c r="O4">
+        <v>6128444</v>
+      </c>
+      <c r="P4">
+        <v>6128444</v>
+      </c>
+      <c r="Q4">
+        <v>16913448.829999998</v>
+      </c>
+      <c r="R4">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="H3">
-        <v>0.7</v>
-      </c>
-      <c r="I3">
-        <v>0.25</v>
-      </c>
-      <c r="J3">
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>2018</v>
+      </c>
+      <c r="L5">
+        <v>2030</v>
+      </c>
+      <c r="M5">
         <v>2019</v>
       </c>
-      <c r="K3">
-        <v>2030</v>
-      </c>
-      <c r="L3">
-        <v>2019</v>
-      </c>
-      <c r="M3">
+      <c r="N5">
+        <v>2023</v>
+      </c>
+      <c r="O5">
         <v>6128444</v>
       </c>
-      <c r="N3">
+      <c r="P5">
         <v>6128444</v>
       </c>
-      <c r="O3">
+      <c r="Q5">
         <v>16913448.829999998</v>
       </c>
-      <c r="P3">
+      <c r="R5">
         <v>0.1</v>
       </c>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>2018</v>
-      </c>
-      <c r="K4">
-        <v>2030</v>
-      </c>
-      <c r="L4">
-        <v>2019</v>
-      </c>
-      <c r="M4">
-        <v>6128444</v>
-      </c>
-      <c r="N4">
-        <v>6128444</v>
-      </c>
-      <c r="O4">
-        <v>16913448.829999998</v>
-      </c>
-      <c r="P4">
-        <v>0.1</v>
+      <c r="S5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -989,6 +1113,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100DEE3DD05F1781645A88261586288E143" ma:contentTypeVersion="8" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="10141bd3b7df6929ac2aab0d38ace983">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84fd47fe-9509-4b60-beed-e31c94bc7d6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="679635ba64e6b0b974d32fba01d99d42" ns2:_="">
     <xsd:import namespace="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
@@ -1160,7 +1290,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1169,20 +1299,37 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ WWF-Sweden/ITR-tool@1685c9af8c5d806845538a4418a853847317df7a 🚀
</commit_message>
<xml_diff>
--- a/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
+++ b/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27716"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mountainrambler\ITR\ITR-tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE29F8-0C6F-4264-AD05-34045B75FE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4843A205-7D81-4F84-856B-56B0E2D2FDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46485" yWindow="3765" windowWidth="32310" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29295" yWindow="2325" windowWidth="28410" windowHeight="13830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
   <si>
     <t>company_name</t>
   </si>
@@ -226,6 +226,66 @@
   </si>
   <si>
     <t>s3_category</t>
+  </si>
+  <si>
+    <t>ghg_s3_1</t>
+  </si>
+  <si>
+    <t>ghg_s3_2</t>
+  </si>
+  <si>
+    <t>ghg_s3_3</t>
+  </si>
+  <si>
+    <t>ghg_s3_4</t>
+  </si>
+  <si>
+    <t>ghg_s3_5</t>
+  </si>
+  <si>
+    <t>ghg_s3_6</t>
+  </si>
+  <si>
+    <t>ghg_s3_7</t>
+  </si>
+  <si>
+    <t>ghg_s3_8</t>
+  </si>
+  <si>
+    <t>ghg_s3_9</t>
+  </si>
+  <si>
+    <t>ghg_s3_10</t>
+  </si>
+  <si>
+    <t>ghg_s3_11</t>
+  </si>
+  <si>
+    <t>ghg_s3_12</t>
+  </si>
+  <si>
+    <t>ghg_s3_13</t>
+  </si>
+  <si>
+    <t>ghg_s3_14</t>
+  </si>
+  <si>
+    <t>ghg_s3_15</t>
+  </si>
+  <si>
+    <t>S1+S3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T_score</t>
+  </si>
+  <si>
+    <t>base_year_ts</t>
+  </si>
+  <si>
+    <t>end_year_ts</t>
   </si>
 </sst>
 </file>
@@ -308,9 +368,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R51" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:R51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AG51" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:AG51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="isic"/>
@@ -329,19 +389,36 @@
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="company_enterprise_value"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="company_total_assets" dataDxfId="0"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="company_cash_equivalents"/>
+    <tableColumn id="15" xr3:uid="{256BCA52-9280-4997-A9FA-121BDEC5100B}" name="ghg_s3_1"/>
+    <tableColumn id="16" xr3:uid="{8E5A0946-C1AF-4AE4-A510-68C7ADE3F0F2}" name="ghg_s3_2"/>
+    <tableColumn id="17" xr3:uid="{CACCEB89-155A-4898-9D90-2A3D13BFA3C7}" name="ghg_s3_3"/>
+    <tableColumn id="19" xr3:uid="{CD17B383-9125-40A3-9BFA-812C473FC022}" name="ghg_s3_4"/>
+    <tableColumn id="23" xr3:uid="{C9F16B44-BF5B-499A-ABEF-2B18736D305C}" name="ghg_s3_5"/>
+    <tableColumn id="24" xr3:uid="{3C1C03F1-4839-4665-BD5F-41FC063718A5}" name="ghg_s3_6"/>
+    <tableColumn id="25" xr3:uid="{9131170B-C6FD-46FB-A114-AE2FDAD29E3D}" name="ghg_s3_7"/>
+    <tableColumn id="26" xr3:uid="{9F7254FA-24DF-4466-8355-697B45B950B2}" name="ghg_s3_8"/>
+    <tableColumn id="27" xr3:uid="{70EFCED7-D284-4EFE-AFE8-6F1FED3EFB5C}" name="ghg_s3_9"/>
+    <tableColumn id="28" xr3:uid="{C305DCD9-AF97-4565-B594-BC14113A345A}" name="ghg_s3_10"/>
+    <tableColumn id="29" xr3:uid="{E9B4C03E-468A-42A5-9D4A-EE5F8160464D}" name="ghg_s3_11"/>
+    <tableColumn id="30" xr3:uid="{EA538E42-F495-439E-A026-0A1A17ABFA08}" name="ghg_s3_12"/>
+    <tableColumn id="31" xr3:uid="{0291F357-5039-4DED-9374-035F6976E89A}" name="ghg_s3_13"/>
+    <tableColumn id="32" xr3:uid="{09FFED3C-FB70-4B86-A27D-FFC96A3EE88C}" name="ghg_s3_14"/>
+    <tableColumn id="33" xr3:uid="{1FE8C48A-9F10-4676-9E25-91FD00A99713}" name="ghg_s3_15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:S121" totalsRowShown="0">
-  <autoFilter ref="A1:S121" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:U121" totalsRowShown="0">
+  <autoFilter ref="A1:U121" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="target_type"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="intensity_metric"/>
+    <tableColumn id="20" xr3:uid="{074AA831-FB43-434C-B38F-8A8281BE4D03}" name="base_year_ts"/>
+    <tableColumn id="21" xr3:uid="{64672385-9C17-450D-A4F7-BA3989DEC2F2}" name="end_year_ts"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="scope"/>
     <tableColumn id="19" xr3:uid="{9248934B-75D3-4E38-B527-74646CCCA9CA}" name="s3_category"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="coverage_s1"/>
@@ -625,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,9 +719,10 @@
     <col min="16" max="16" width="28" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="33" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,8 +777,53 @@
       <c r="R1" t="s">
         <v>15</v>
       </c>
+      <c r="S1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -755,8 +878,17 @@
       <c r="R2">
         <v>990719858</v>
       </c>
+      <c r="Y2">
+        <v>3033133</v>
+      </c>
+      <c r="AC2">
+        <v>55000</v>
+      </c>
+      <c r="AG2">
+        <v>58800000</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -813,6 +945,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -823,10 +956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,16 +967,17 @@
     <col min="1" max="1" width="17.109375" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="4" width="21.109375" customWidth="1"/>
-    <col min="7" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
-    <col min="13" max="14" width="21" customWidth="1"/>
-    <col min="15" max="17" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14" customWidth="1"/>
+    <col min="9" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" customWidth="1"/>
+    <col min="15" max="16" width="21" customWidth="1"/>
+    <col min="17" max="19" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -857,52 +991,58 @@
         <v>35</v>
       </c>
       <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>42</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>54</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>44</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>46</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>47</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -912,44 +1052,44 @@
       <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.95</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.95</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>0.35</v>
-      </c>
-      <c r="K2">
-        <v>2020</v>
-      </c>
-      <c r="L2">
-        <v>2035</v>
       </c>
       <c r="M2">
         <v>2020</v>
       </c>
       <c r="N2">
+        <v>2035</v>
+      </c>
+      <c r="O2">
+        <v>2020</v>
+      </c>
+      <c r="P2">
         <v>2024</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>458332160</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>61888133</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>0</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -962,47 +1102,47 @@
       <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>52</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0.7</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>0.25</v>
-      </c>
-      <c r="K3">
-        <v>2019</v>
-      </c>
-      <c r="L3">
-        <v>2030</v>
       </c>
       <c r="M3">
         <v>2019</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3">
+        <v>2030</v>
+      </c>
+      <c r="O3">
+        <v>2019</v>
+      </c>
+      <c r="P3" s="2">
         <v>45200</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>6128444</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>6128444</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>16913448.829999998</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>0.1</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1012,44 +1152,44 @@
       <c r="C4" t="s">
         <v>48</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>59</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.85</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>0.5</v>
-      </c>
-      <c r="K4">
-        <v>2019</v>
-      </c>
-      <c r="L4">
-        <v>2030</v>
       </c>
       <c r="M4">
         <v>2019</v>
       </c>
       <c r="N4">
+        <v>2030</v>
+      </c>
+      <c r="O4">
+        <v>2019</v>
+      </c>
+      <c r="P4">
         <v>2024</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>6128444</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>6128444</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>16913448.829999998</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>0.1</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1062,44 +1202,100 @@
       <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>49</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>5</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>2018</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>2030</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>2019</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>2023</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>6128444</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>6128444</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>16913448.829999998</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>0.1</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6">
+        <v>3.2</v>
+      </c>
+      <c r="F6">
+        <v>2.4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>2018</v>
+      </c>
+      <c r="N6">
+        <v>2030</v>
+      </c>
+      <c r="O6">
+        <v>2019</v>
+      </c>
+      <c r="P6">
+        <v>2023</v>
+      </c>
+      <c r="Q6">
+        <v>6128444</v>
+      </c>
+      <c r="R6">
+        <v>6128444</v>
+      </c>
+      <c r="S6">
+        <v>16913448.829999998</v>
+      </c>
+      <c r="T6">
+        <v>0.1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1119,6 +1315,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100DEE3DD05F1781645A88261586288E143" ma:contentTypeVersion="8" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="10141bd3b7df6929ac2aab0d38ace983">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84fd47fe-9509-4b60-beed-e31c94bc7d6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="679635ba64e6b0b974d32fba01d99d42" ns2:_="">
     <xsd:import namespace="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
@@ -1290,15 +1495,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}">
   <ds:schemaRefs>
@@ -1309,6 +1505,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1324,12 +1528,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ WWF-Sweden/ITR-tool@2ed80dcb73efcf5b36f5e9aaffc05bea83c68af8 🚀
</commit_message>
<xml_diff>
--- a/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
+++ b/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27716"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mountainrambler\ITR\ITR-tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4843A205-7D81-4F84-856B-56B0E2D2FDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A274C8-5821-4F53-B95B-901831610354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="2325" windowWidth="28410" windowHeight="13830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30225" yWindow="4470" windowWidth="28800" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="89">
   <si>
     <t>company_name</t>
   </si>
@@ -273,9 +273,6 @@
     <t>ghg_s3_15</t>
   </si>
   <si>
-    <t>S1+S3</t>
-  </si>
-  <si>
     <t>T4</t>
   </si>
   <si>
@@ -286,6 +283,24 @@
   </si>
   <si>
     <t>end_year_ts</t>
+  </si>
+  <si>
+    <t>ghg_s1s2</t>
+  </si>
+  <si>
+    <t>base_year_ghg_s1s2</t>
+  </si>
+  <si>
+    <t>C_1</t>
+  </si>
+  <si>
+    <t>C_2</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>Int_to_abs</t>
   </si>
 </sst>
 </file>
@@ -368,9 +383,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AG51" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:AG51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AH41" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:AH41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="isic"/>
@@ -383,6 +398,7 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="sector"/>
     <tableColumn id="14" xr3:uid="{4E3A16A5-1D49-4E34-85C1-76B963C0C39B}" name="ghg_s1"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ghg_s2"/>
+    <tableColumn id="34" xr3:uid="{7E7DBEA7-A974-4FC0-A3C7-534274C4D0E4}" name="ghg_s1s2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ghg_s3"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="company_revenue"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="company_market_cap"/>
@@ -410,9 +426,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:U121" totalsRowShown="0">
-  <autoFilter ref="A1:U121" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:V121" totalsRowShown="0">
+  <autoFilter ref="A1:V121" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="target_type"/>
@@ -431,6 +447,7 @@
     <tableColumn id="17" xr3:uid="{402ACC87-EC14-4797-B51B-7DC99260B94B}" name="statement_date"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="base_year_ghg_s1"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="base_year_ghg_s2"/>
+    <tableColumn id="22" xr3:uid="{86F15313-E77B-4ED9-B753-3C4AFFA53386}" name="base_year_ghg_s1s2"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="base_year_ghg_s3"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="achieved_reduction"/>
     <tableColumn id="18" xr3:uid="{9D6E6BD8-AF52-471F-81F4-E934F549E268}" name="target_ids"/>
@@ -702,27 +719,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AL6" sqref="AL6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="21.5546875" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="33" width="11.21875" customWidth="1"/>
+    <col min="3" max="13" width="21.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="34" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -760,75 +777,78 @@
         <v>62</v>
       </c>
       <c r="M1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>64</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>65</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>66</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>67</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>68</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>70</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>71</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>72</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>73</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>74</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>75</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>76</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>77</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -861,39 +881,42 @@
         <v>188332160</v>
       </c>
       <c r="M2">
+        <v>416664320</v>
+      </c>
+      <c r="N2">
         <v>61888133</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>7370536918</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>7318942238</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>24392175674</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>21337139</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>990719858</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>3033133</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>55000</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>58800000</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -926,22 +949,37 @@
         <v>3266889</v>
       </c>
       <c r="M3">
+        <v>16533778.880000001</v>
+      </c>
+      <c r="N3">
         <v>18413448.829999998</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>2795781568</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>3615211346</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>3620291185</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>43581896.049999997</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>463981837.19999999</v>
+      </c>
+      <c r="U3">
+        <v>2250550</v>
+      </c>
+      <c r="W3">
+        <v>588899</v>
+      </c>
+      <c r="AB3">
+        <v>588778</v>
+      </c>
+      <c r="AE3">
+        <v>121255</v>
       </c>
     </row>
   </sheetData>
@@ -956,10 +994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,11 +1011,14 @@
     <col min="13" max="13" width="12.109375" customWidth="1"/>
     <col min="14" max="14" width="11.44140625" customWidth="1"/>
     <col min="15" max="16" width="21" customWidth="1"/>
-    <col min="17" max="19" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.88671875" customWidth="1"/>
+    <col min="20" max="20" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -991,10 +1032,10 @@
         <v>35</v>
       </c>
       <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -1033,21 +1074,24 @@
         <v>45</v>
       </c>
       <c r="S1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" t="s">
         <v>46</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>47</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
@@ -1082,19 +1126,22 @@
       <c r="R2">
         <v>61888133</v>
       </c>
-      <c r="T2">
+      <c r="S2">
+        <v>61888133</v>
+      </c>
+      <c r="U2">
         <v>0</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>85</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
@@ -1133,21 +1180,24 @@
         <v>6128444</v>
       </c>
       <c r="S3">
+        <v>6128444</v>
+      </c>
+      <c r="T3">
         <v>16913448.829999998</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>0.1</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -1180,21 +1230,24 @@
         <v>6128444</v>
       </c>
       <c r="S4">
+        <v>6128444</v>
+      </c>
+      <c r="T4">
         <v>16913448.829999998</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>0.1</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5">
-        <v>2</v>
+      <c r="B5" t="s">
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
@@ -1212,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="M5">
         <v>2018</v>
@@ -1233,24 +1286,27 @@
         <v>6128444</v>
       </c>
       <c r="S5">
+        <v>6128444</v>
+      </c>
+      <c r="T5">
         <v>16913448.829999998</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>0.1</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="B6" t="s">
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6">
         <v>3.2</v>
@@ -1259,16 +1315,10 @@
         <v>2.4</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="L6">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="M6">
         <v>2018</v>
@@ -1289,13 +1339,69 @@
         <v>6128444</v>
       </c>
       <c r="S6">
+        <v>6128444</v>
+      </c>
+      <c r="T6">
         <v>16913448.829999998</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>0.1</v>
       </c>
-      <c r="U6" t="s">
-        <v>80</v>
+      <c r="V6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0.7</v>
+      </c>
+      <c r="M7">
+        <v>2018</v>
+      </c>
+      <c r="N7">
+        <v>2030</v>
+      </c>
+      <c r="O7">
+        <v>2019</v>
+      </c>
+      <c r="P7">
+        <v>2023</v>
+      </c>
+      <c r="Q7">
+        <v>6128444</v>
+      </c>
+      <c r="R7">
+        <v>6128444</v>
+      </c>
+      <c r="S7">
+        <v>6128444</v>
+      </c>
+      <c r="T7">
+        <v>16913448.829999998</v>
+      </c>
+      <c r="U7">
+        <v>0.1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1309,12 +1415,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1323,7 +1423,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100DEE3DD05F1781645A88261586288E143" ma:contentTypeVersion="8" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="10141bd3b7df6929ac2aab0d38ace983">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84fd47fe-9509-4b60-beed-e31c94bc7d6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="679635ba64e6b0b974d32fba01d99d42" ns2:_="">
     <xsd:import namespace="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
@@ -1495,16 +1595,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1512,7 +1609,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1528,4 +1625,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>